<commit_message>
finished assigment week 10
</commit_message>
<xml_diff>
--- a/week10/implicit evaluations study/data/processed/data_processed_codebook.xlsx
+++ b/week10/implicit evaluations study/data/processed/data_processed_codebook.xlsx
@@ -1,76 +1,122 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szuki\git\dmp-assignments\week10\implicit evaluations study\data\processed\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6640C9D6-7869-4263-9207-296BE957D00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">explanation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">like</t>
-  </si>
-  <si>
-    <t xml:space="preserve">positive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_evaluation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMP_score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proportion_fast_trials_amp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude_amp_performance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude_amp_completeness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude_duplicate_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude_participant</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>prefer</t>
+  </si>
+  <si>
+    <t>mean_evaluation</t>
+  </si>
+  <si>
+    <t>AMP_score</t>
+  </si>
+  <si>
+    <t>proportion_fast_trials_amp</t>
+  </si>
+  <si>
+    <t>exclude_amp_performance</t>
+  </si>
+  <si>
+    <t>exclude_amp_completeness</t>
+  </si>
+  <si>
+    <t>exclude_duplicate_data</t>
+  </si>
+  <si>
+    <t>exclude_participant</t>
+  </si>
+  <si>
+    <t>Day of testing</t>
+  </si>
+  <si>
+    <t>time of testing</t>
+  </si>
+  <si>
+    <t>Age of the subject in years</t>
+  </si>
+  <si>
+    <t>Identified gender of participant</t>
+  </si>
+  <si>
+    <t>unique identification number for each subject</t>
+  </si>
+  <si>
+    <t>mean of self report evaluation</t>
+  </si>
+  <si>
+    <t>AMP score of participant</t>
+  </si>
+  <si>
+    <t>proportion of trials that were faster than 100 miliseconds</t>
+  </si>
+  <si>
+    <t>participant to be excluded if amp response is below 100 miliseconds</t>
+  </si>
+  <si>
+    <t>exclude if participants has more or less than 72 data rows</t>
+  </si>
+  <si>
+    <t>exclude duplicate data of participants</t>
+  </si>
+  <si>
+    <t>participants to be excluded if demographics or outcome measures are missing</t>
+  </si>
+  <si>
+    <t>Item and its response</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,6 +152,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -387,14 +442,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,98 +462,128 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2"/>
-    </row>
-    <row r="3">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3"/>
-    </row>
-    <row r="4">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4"/>
-    </row>
-    <row r="5">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5"/>
-    </row>
-    <row r="6">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6"/>
-    </row>
-    <row r="7">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7"/>
-    </row>
-    <row r="8">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8"/>
-    </row>
-    <row r="9">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9"/>
-    </row>
-    <row r="10">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10"/>
-    </row>
-    <row r="11">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11"/>
-    </row>
-    <row r="12">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12"/>
-    </row>
-    <row r="13">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13"/>
-    </row>
-    <row r="14">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14"/>
-    </row>
-    <row r="15">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15"/>
-    </row>
-    <row r="16">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16"/>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>